<commit_message>
Revert "my third commin"
</commit_message>
<xml_diff>
--- a/Check_list.xlsx
+++ b/Check_list.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="525" windowWidth="10455" windowHeight="12375" activeTab="1"/>
+    <workbookView xWindow="750" yWindow="525" windowWidth="10455" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="152">
   <si>
     <t>Epic-1: Базовые вычисления и логика</t>
   </si>
@@ -668,14 +667,6 @@
       <t>В процессе тестирования (Not Run)</t>
     </r>
   </si>
-  <si>
-    <t>안녕하세요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>저는 아나스타샤예요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
@@ -684,7 +675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -748,14 +739,6 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -897,7 +880,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -941,27 +924,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -969,7 +931,27 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1191,8 +1173,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1207,38 +1189,38 @@
     <row r="1" spans="1:8" ht="16.5">
       <c r="A1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="16.5">
       <c r="A2" s="1"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="6" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:8" ht="16.5">
       <c r="A4" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="16.5">
       <c r="A5" s="6" t="s">
@@ -1305,16 +1287,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="38.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="9">
         <v>46023</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -1595,7 +1577,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15">
-      <c r="A28" s="24"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="11" t="s">
         <v>46</v>
       </c>
@@ -1619,7 +1601,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="12">
@@ -1885,7 +1867,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="25" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="14">
@@ -2079,7 +2061,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15">
-      <c r="A48" s="24"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="14">
         <v>46237</v>
       </c>
@@ -2103,7 +2085,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="15">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B49" s="16">
@@ -2585,7 +2567,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="15">
-      <c r="A69" s="24"/>
+      <c r="A69" s="23"/>
       <c r="B69" s="18" t="s">
         <v>140</v>
       </c>
@@ -2623,33 +2605,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "my third commin""
</commit_message>
<xml_diff>
--- a/Check_list.xlsx
+++ b/Check_list.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="525" windowWidth="10455" windowHeight="12375"/>
+    <workbookView xWindow="750" yWindow="525" windowWidth="10455" windowHeight="12375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="154">
   <si>
     <t>Epic-1: Базовые вычисления и логика</t>
   </si>
@@ -667,6 +668,14 @@
       <t>В процессе тестирования (Not Run)</t>
     </r>
   </si>
+  <si>
+    <t>안녕하세요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저는 아나스타샤예요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -675,7 +684,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -739,6 +748,14 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -880,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -924,6 +941,27 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -931,27 +969,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1173,8 +1191,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1189,38 +1207,38 @@
     <row r="1" spans="1:8" ht="16.5">
       <c r="A1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="16.5">
       <c r="A2" s="1"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="6" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="16.5">
       <c r="A4" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="20"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:8" ht="16.5">
       <c r="A5" s="6" t="s">
@@ -1287,16 +1305,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="38.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="9">
         <v>46023</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -1577,7 +1595,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="11" t="s">
         <v>46</v>
       </c>
@@ -1601,7 +1619,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="12">
@@ -1867,7 +1885,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="23" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="14">
@@ -2061,7 +2079,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15">
-      <c r="A48" s="23"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="14">
         <v>46237</v>
       </c>
@@ -2085,7 +2103,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="15">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="25" t="s">
         <v>91</v>
       </c>
       <c r="B49" s="16">
@@ -2567,7 +2585,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="15">
-      <c r="A69" s="23"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="18" t="s">
         <v>140</v>
       </c>
@@ -2605,4 +2623,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>